<commit_message>
extract data from spreadsheet
</commit_message>
<xml_diff>
--- a/web/public/Trash-Data-Template.xlsx
+++ b/web/public/Trash-Data-Template.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Cleanup Details</t>
   </si>
@@ -38,12 +38,18 @@
     <t>Trash Data</t>
   </si>
   <si>
+    <t>Everything is optional.</t>
+  </si>
+  <si>
     <t>Total Weight (kg)</t>
   </si>
   <si>
     <t>Total weight of all items collected</t>
   </si>
   <si>
+    <t>Number of Trash Bags Used</t>
+  </si>
+  <si>
     <t>Cans</t>
   </si>
   <si>
@@ -56,18 +62,18 @@
     <t>Large blue/white/grey water drums</t>
   </si>
   <si>
+    <t>Electronics</t>
+  </si>
+  <si>
+    <t>e.g. light bulbs, batteries, phones, circuitboards</t>
+  </si>
+  <si>
+    <t>Footwear</t>
+  </si>
+  <si>
     <t>Glass</t>
   </si>
   <si>
-    <t>Electronics</t>
-  </si>
-  <si>
-    <t>e.g. light bulbs, batteries, phones, circuitboards</t>
-  </si>
-  <si>
-    <t>Footwear</t>
-  </si>
-  <si>
     <t>Jerry Cans</t>
   </si>
   <si>
@@ -84,6 +90,9 @@
   </si>
   <si>
     <t>e.g. cigarette lighters, cigarette buts</t>
+  </si>
+  <si>
+    <t>Tires</t>
   </si>
   <si>
     <t>Other Items</t>
@@ -535,7 +544,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.63"/>
+    <col customWidth="1" min="1" max="1" width="24.0"/>
     <col customWidth="1" min="2" max="2" width="20.0"/>
     <col customWidth="1" min="3" max="3" width="2.5"/>
     <col customWidth="1" min="4" max="4" width="57.0"/>
@@ -590,28 +599,28 @@
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9">
       <c r="D9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5"/>
       <c r="D10" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="5"/>
-      <c r="D11" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="D11" s="6"/>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
@@ -627,55 +636,55 @@
         <v>14</v>
       </c>
       <c r="B13" s="5"/>
-      <c r="D13" s="2"/>
+      <c r="D13" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" s="5"/>
       <c r="D14" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15" s="5"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="5"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17" s="5"/>
-      <c r="D17" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="D17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="5"/>
-      <c r="D18" s="2"/>
+      <c r="D18" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19" s="5"/>
-      <c r="D19" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="D19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
@@ -687,10 +696,20 @@
       </c>
     </row>
     <row r="21">
-      <c r="D21" s="2"/>
+      <c r="A21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="D21" s="6"/>
     </row>
     <row r="22">
-      <c r="D22" s="2"/>
+      <c r="A22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="D22" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="23">
       <c r="D23" s="2"/>
@@ -3632,10 +3651,16 @@
     <row r="1002">
       <c r="D1002" s="2"/>
     </row>
+    <row r="1003">
+      <c r="D1003" s="2"/>
+    </row>
+    <row r="1004">
+      <c r="D1004" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B5">
@@ -3661,7 +3686,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -3691,207 +3716,207 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>